<commit_message>
revised- corrected 2019 input
</commit_message>
<xml_diff>
--- a/descriptives/micro_age_sex_table_2015_2024.xlsx
+++ b/descriptives/micro_age_sex_table_2015_2024.xlsx
@@ -7227,10 +7227,10 @@
         </is>
       </c>
       <c r="D206" t="n">
-        <v>3104.576347994024</v>
+        <v>3104.576347994023</v>
       </c>
       <c r="E206" t="n">
-        <v>341.5033982793426</v>
+        <v>341.5033982793425</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
@@ -7263,7 +7263,7 @@
         <v>13492.53591776149</v>
       </c>
       <c r="E207" t="n">
-        <v>1484.178950953764</v>
+        <v>1484.178950953763</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
@@ -7302,10 +7302,10 @@
         <v>0</v>
       </c>
       <c r="G208" t="n">
-        <v>23028.64341137492</v>
+        <v>23028.64341137491</v>
       </c>
       <c r="H208" t="n">
-        <v>2533.150775251241</v>
+        <v>2533.15077525124</v>
       </c>
       <c r="I208" t="n">
         <v>0</v>
@@ -7329,16 +7329,16 @@
         <v>3454.760863945289</v>
       </c>
       <c r="E209" t="n">
-        <v>380.0236950339819</v>
+        <v>380.0236950339818</v>
       </c>
       <c r="F209" t="n">
         <v>0</v>
       </c>
       <c r="G209" t="n">
-        <v>3110.382928734727</v>
+        <v>3110.382928734726</v>
       </c>
       <c r="H209" t="n">
-        <v>342.14212216082</v>
+        <v>342.1421221608198</v>
       </c>
       <c r="I209" t="n">
         <v>0</v>
@@ -7359,7 +7359,7 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>14089.96798487008</v>
+        <v>14089.96798487007</v>
       </c>
       <c r="E210" t="n">
         <v>1549.896478335709</v>
@@ -7401,10 +7401,10 @@
         <v>0</v>
       </c>
       <c r="G211" t="n">
-        <v>33683.36392853006</v>
+        <v>33683.36392853005</v>
       </c>
       <c r="H211" t="n">
-        <v>3705.170032138306</v>
+        <v>3705.170032138305</v>
       </c>
       <c r="I211" t="n">
         <v>0</v>
@@ -7425,19 +7425,19 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>3455.955202026501</v>
+        <v>3455.9552020265</v>
       </c>
       <c r="E212" t="n">
-        <v>380.1550722229151</v>
+        <v>380.155072222915</v>
       </c>
       <c r="F212" t="n">
         <v>0</v>
       </c>
       <c r="G212" t="n">
-        <v>3515.812352751398</v>
+        <v>3515.812352751397</v>
       </c>
       <c r="H212" t="n">
-        <v>386.7393588026538</v>
+        <v>386.7393588026537</v>
       </c>
       <c r="I212" t="n">
         <v>0</v>
@@ -7458,7 +7458,7 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>14502.992700191</v>
+        <v>14502.99270019099</v>
       </c>
       <c r="E213" t="n">
         <v>1595.32919702101</v>
@@ -7470,7 +7470,7 @@
         <v>14567.51648454345</v>
       </c>
       <c r="H213" t="n">
-        <v>1602.42681329978</v>
+        <v>1602.426813299779</v>
       </c>
       <c r="I213" t="n">
         <v>0</v>
@@ -7500,10 +7500,10 @@
         <v>0</v>
       </c>
       <c r="G214" t="n">
-        <v>29420.79837956577</v>
+        <v>29420.79837956576</v>
       </c>
       <c r="H214" t="n">
-        <v>3236.287821752234</v>
+        <v>3236.287821752233</v>
       </c>
       <c r="I214" t="n">
         <v>0</v>
@@ -7527,7 +7527,7 @@
         <v>3300.057481240814</v>
       </c>
       <c r="E215" t="n">
-        <v>363.0063229364896</v>
+        <v>363.0063229364895</v>
       </c>
       <c r="F215" t="n">
         <v>0</v>
@@ -7560,7 +7560,7 @@
         <v>15209.92401110448</v>
       </c>
       <c r="E216" t="n">
-        <v>1673.091641221493</v>
+        <v>1673.091641221492</v>
       </c>
       <c r="F216" t="n">
         <v>0</v>
@@ -7590,7 +7590,7 @@
         </is>
       </c>
       <c r="D217" t="n">
-        <v>30704.35133443289</v>
+        <v>30704.35133443288</v>
       </c>
       <c r="E217" t="n">
         <v>3377.478646787617</v>
@@ -7602,7 +7602,7 @@
         <v>26125.21476150972</v>
       </c>
       <c r="H217" t="n">
-        <v>2873.77362376607</v>
+        <v>2873.773623766069</v>
       </c>
       <c r="I217" t="n">
         <v>0</v>
@@ -7623,7 +7623,7 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>3436.019810561763</v>
+        <v>3436.019810561762</v>
       </c>
       <c r="E218" t="n">
         <v>377.9621791617939</v>
@@ -7632,7 +7632,7 @@
         <v>0</v>
       </c>
       <c r="G218" t="n">
-        <v>3605.353734803219</v>
+        <v>3605.353734803218</v>
       </c>
       <c r="H218" t="n">
         <v>396.588910828354</v>
@@ -7692,16 +7692,16 @@
         <v>27449.42793604665</v>
       </c>
       <c r="E220" t="n">
-        <v>3019.437072965132</v>
+        <v>3019.437072965131</v>
       </c>
       <c r="F220" t="n">
         <v>0</v>
       </c>
       <c r="G220" t="n">
-        <v>28200.54387419741</v>
+        <v>28200.5438741974</v>
       </c>
       <c r="H220" t="n">
-        <v>3102.059826161716</v>
+        <v>3102.059826161715</v>
       </c>
       <c r="I220" t="n">
         <v>0</v>
@@ -7722,16 +7722,16 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>3641.218282405088</v>
+        <v>3641.218282405087</v>
       </c>
       <c r="E221" t="n">
-        <v>400.5340110645596</v>
+        <v>400.5340110645595</v>
       </c>
       <c r="F221" t="n">
         <v>0</v>
       </c>
       <c r="G221" t="n">
-        <v>2787.360281972002</v>
+        <v>2787.360281972001</v>
       </c>
       <c r="H221" t="n">
         <v>306.6096310169202</v>
@@ -7755,10 +7755,10 @@
         </is>
       </c>
       <c r="D222" t="n">
-        <v>13723.7072572589</v>
+        <v>13723.70725725889</v>
       </c>
       <c r="E222" t="n">
-        <v>1509.607798298479</v>
+        <v>1509.607798298478</v>
       </c>
       <c r="F222" t="n">
         <v>0</v>
@@ -7788,7 +7788,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>26656.44940800742</v>
+        <v>26656.44940800741</v>
       </c>
       <c r="E223" t="n">
         <v>2932.209434880816</v>
@@ -7797,10 +7797,10 @@
         <v>0</v>
       </c>
       <c r="G223" t="n">
-        <v>25225.88362235106</v>
+        <v>25225.88362235105</v>
       </c>
       <c r="H223" t="n">
-        <v>2774.847198458616</v>
+        <v>2774.847198458615</v>
       </c>
       <c r="I223" t="n">
         <v>0</v>
@@ -7821,19 +7821,19 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>3005.132428124713</v>
+        <v>3005.132428124712</v>
       </c>
       <c r="E224" t="n">
-        <v>330.5645670937184</v>
+        <v>330.5645670937183</v>
       </c>
       <c r="F224" t="n">
         <v>0</v>
       </c>
       <c r="G224" t="n">
-        <v>3290.846703294849</v>
+        <v>3290.846703294848</v>
       </c>
       <c r="H224" t="n">
-        <v>361.9931373624335</v>
+        <v>361.9931373624333</v>
       </c>
       <c r="I224" t="n">
         <v>0</v>
@@ -7854,7 +7854,7 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>13491.44210161737</v>
+        <v>13491.44210161736</v>
       </c>
       <c r="E225" t="n">
         <v>1484.05863117791</v>
@@ -7863,7 +7863,7 @@
         <v>0</v>
       </c>
       <c r="G225" t="n">
-        <v>12980.19787221751</v>
+        <v>12980.1978722175</v>
       </c>
       <c r="H225" t="n">
         <v>1427.821765943926</v>
@@ -7890,16 +7890,16 @@
         <v>26633.88146567381</v>
       </c>
       <c r="E226" t="n">
-        <v>2929.72696122412</v>
+        <v>2929.726961224119</v>
       </c>
       <c r="F226" t="n">
         <v>0</v>
       </c>
       <c r="G226" t="n">
-        <v>24020.75345078371</v>
+        <v>24020.7534507837</v>
       </c>
       <c r="H226" t="n">
-        <v>2642.282879586208</v>
+        <v>2642.282879586207</v>
       </c>
       <c r="I226" t="n">
         <v>0</v>
@@ -7920,10 +7920,10 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>3626.385309308662</v>
+        <v>3626.385309308661</v>
       </c>
       <c r="E227" t="n">
-        <v>398.9023840239528</v>
+        <v>398.9023840239527</v>
       </c>
       <c r="F227" t="n">
         <v>0</v>
@@ -7953,7 +7953,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>15514.60586411838</v>
+        <v>15514.60586411837</v>
       </c>
       <c r="E228" t="n">
         <v>1706.606645053021</v>
@@ -7998,7 +7998,7 @@
         <v>26076.85781058708</v>
       </c>
       <c r="H229" t="n">
-        <v>2868.454359164579</v>
+        <v>2868.454359164578</v>
       </c>
       <c r="I229" t="n">
         <v>0</v>
@@ -8019,10 +8019,10 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>3788.15656503382</v>
+        <v>3788.156565033819</v>
       </c>
       <c r="E230" t="n">
-        <v>416.6972221537202</v>
+        <v>416.6972221537201</v>
       </c>
       <c r="F230" t="n">
         <v>0</v>
@@ -8055,7 +8055,7 @@
         <v>14182.44888363586</v>
       </c>
       <c r="E231" t="n">
-        <v>1560.069377199945</v>
+        <v>1560.069377199944</v>
       </c>
       <c r="F231" t="n">
         <v>0</v>
@@ -8085,7 +8085,7 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>32102.21397401952</v>
+        <v>32102.21397401951</v>
       </c>
       <c r="E232" t="n">
         <v>3531.243537142147</v>

</xml_diff>